<commit_message>
Working app for Render
</commit_message>
<xml_diff>
--- a/data/responses.xlsx
+++ b/data/responses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>Address</t>
   </si>
@@ -145,12 +145,18 @@
     <t>wire_dia</t>
   </si>
   <si>
+    <t>Rate per Hour</t>
+  </si>
+  <si>
     <t>Coimbatore</t>
   </si>
   <si>
     <t>kaizen</t>
   </si>
   <si>
+    <t>kaixwn</t>
+  </si>
+  <si>
     <t>Conventional Milling</t>
   </si>
   <si>
@@ -161,12 +167,6 @@
   </si>
   <si>
     <t>Wire Electrical Discharge Machining</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>100</t>
   </si>
   <si>
     <t>M2</t>
@@ -563,13 +563,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ5"/>
+  <dimension ref="A1:AR7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:44">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,16 +699,19 @@
       <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="AR1" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:44">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -741,15 +744,15 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:44">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -782,21 +785,21 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:44">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
         <v>49</v>
       </c>
-      <c r="E4" t="s">
-        <v>50</v>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
       </c>
       <c r="F4" t="s">
         <v>52</v>
@@ -807,37 +810,37 @@
       <c r="H4" t="s">
         <v>57</v>
       </c>
-      <c r="S4" t="s">
-        <v>58</v>
-      </c>
-      <c r="U4" t="s">
-        <v>59</v>
-      </c>
-      <c r="V4" t="s">
-        <v>60</v>
-      </c>
-      <c r="W4" t="s">
-        <v>61</v>
+      <c r="S4">
+        <v>56</v>
+      </c>
+      <c r="U4">
+        <v>12</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>9</v>
       </c>
       <c r="Z4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:44">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s">
         <v>50</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
       </c>
       <c r="F5" t="s">
         <v>51</v>
@@ -848,19 +851,71 @@
       <c r="H5" t="s">
         <v>57</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5">
+        <v>56</v>
+      </c>
+      <c r="U5">
+        <v>12</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>9</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S6">
+        <v>56</v>
+      </c>
+      <c r="U6">
+        <v>12</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>9</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+      <c r="S7" t="s">
         <v>58</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U7" t="s">
         <v>59</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V7" t="s">
         <v>60</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W7" t="s">
         <v>61</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="Z7" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>